<commit_message>
Spalten und Reihen zahlen hinzugefügt
</commit_message>
<xml_diff>
--- a/Example/example_two.xlsx
+++ b/Example/example_two.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Abkürzungen</t>
   </si>
@@ -31,6 +31,15 @@
   </si>
   <si>
     <t xml:space="preserve">adshdaskjhd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hallo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">welcome</t>
   </si>
   <si>
     <t xml:space="preserve">DFA</t>
@@ -137,37 +146,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8520408163265"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>3</v>
+      <c r="A3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -217,7 +239,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="13.0663265306122"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Aufteilung der all Funktion
</commit_message>
<xml_diff>
--- a/Example/example_two.xlsx
+++ b/Example/example_two.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Abkürzungen</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t xml:space="preserve">hi </t>
-  </si>
-  <si>
-    <t xml:space="preserve">welcome</t>
   </si>
   <si>
     <t xml:space="preserve">DFA</t>
@@ -146,7 +143,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -178,18 +175,15 @@
       <c r="D2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>